<commit_message>
Commit and zip. Code edited to match that in analysis.pdf
</commit_message>
<xml_diff>
--- a/analysis/cfu_per_g_d_soil_group3.xlsx
+++ b/analysis/cfu_per_g_d_soil_group3.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobpollard/Desktop/Uni/1.2/BABS-2 /Report and figure/Report/Y3948024/figure_and_stats/data/cfu_per_gram_dry_soil/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobpollard/Desktop/Uni/1.2/BABS-2 /Report and figure/Y3948024/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A6F276-7A63-AD4F-B3EB-F57EC305BE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9439CB-488A-484D-AC37-A90DC9A52FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="680" windowWidth="14180" windowHeight="16020" xr2:uid="{03D709D2-8566-1340-92B8-26B039B141AD}"/>
   </bookViews>
   <sheets>
     <sheet name="g3" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>